<commit_message>
Add new unused positive samples.
</commit_message>
<xml_diff>
--- a/samples/positive/Login Form.xlsx
+++ b/samples/positive/Login Form.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="1174">
   <si>
     <t>Filename</t>
   </si>
@@ -2815,91 +2815,724 @@
     <t>471.html</t>
   </si>
   <si>
+    <t>https://www.handtec.co.uk/account/login</t>
+  </si>
+  <si>
     <t>472.html</t>
   </si>
   <si>
+    <t>https://www.gpscity.com/myaccount</t>
+  </si>
+  <si>
     <t>473.html</t>
   </si>
   <si>
+    <t>https://www.thegpsstore.com/Login.aspx</t>
+  </si>
+  <si>
     <t>474.html</t>
   </si>
   <si>
+    <t>https://gotrack.com/#</t>
+  </si>
+  <si>
     <t>475.html</t>
   </si>
   <si>
+    <t>http://ez.gotrack.com/user/sign_in</t>
+  </si>
+  <si>
     <t>476.html</t>
   </si>
   <si>
+    <t>https://spyassociates.com/login.php</t>
+  </si>
+  <si>
     <t>477.html</t>
   </si>
   <si>
+    <t>https://checkout.na3.netsuite.com/app/center/nlvisitor.nl/c.668948/sc.6/n.1/.f?whence=&amp;ext=T</t>
+  </si>
+  <si>
     <t>478.html</t>
   </si>
   <si>
+    <t>https://www.liveviewgps.net/?cid=LiveViewGPS</t>
+  </si>
+  <si>
     <t>479.html</t>
   </si>
   <si>
+    <t>https://www.gpsnation.com/</t>
+  </si>
+  <si>
     <t>480.html</t>
   </si>
   <si>
+    <t>https://www.navtechgps.com/my_account/login/</t>
+  </si>
+  <si>
     <t>481.html</t>
   </si>
   <si>
+    <t>https://www.cartft.com/common</t>
+  </si>
+  <si>
     <t>482.html</t>
   </si>
   <si>
+    <t>http://gps.rmtracking.com/</t>
+  </si>
+  <si>
     <t>483.html</t>
   </si>
   <si>
+    <t>https://m.rmtracking.com/Account/LogOn?ReturnUrl=%2f</t>
+  </si>
+  <si>
     <t>484.html</t>
   </si>
   <si>
+    <t>https://www.memory-map.co.uk/customer/account/login/referer/aHR0cHM6Ly93d3cubWVtb3J5LW1hcC5jby51ay8_U0lEPXNlZmU4bTRsOG8xZHUzZmxiYW1iNGcxc3Ew/</t>
+  </si>
+  <si>
     <t>485.html</t>
   </si>
   <si>
+    <t>https://www.anchorexpress.com/myaccount.asp</t>
+  </si>
+  <si>
     <t>486.html</t>
   </si>
   <si>
+    <t>https://www.sustuu.com/sign-in.html</t>
+  </si>
+  <si>
     <t>487.html</t>
   </si>
   <si>
+    <t>https://www.gps4us.com/shopcustadminlogin.asp</t>
+  </si>
+  <si>
     <t>488.html</t>
   </si>
   <si>
+    <t>https://shop.gpsoz.com.au/account/login</t>
+  </si>
+  <si>
     <t>489.html</t>
   </si>
   <si>
+    <t>https://www.inventeksys.com/buy-online/my-account/</t>
+  </si>
+  <si>
     <t>490.html</t>
   </si>
   <si>
+    <t>https://speedcams.eu/account</t>
+  </si>
+  <si>
     <t>491.html</t>
   </si>
   <si>
+    <t>https://www.ausluck.com.au/_myacct/login</t>
+  </si>
+  <si>
     <t>492.html</t>
   </si>
   <si>
+    <t>https://buybits.com/customer/account/login/</t>
+  </si>
+  <si>
     <t>493.html</t>
   </si>
   <si>
+    <t>https://gb.snooper.eu/customer/account/login/</t>
+  </si>
+  <si>
     <t>494.html</t>
   </si>
   <si>
+    <t>http://www.navi-tech.co.uk/my-account/</t>
+  </si>
+  <si>
     <t>495.html</t>
   </si>
   <si>
+    <t>http://bigbrotherme.co.nz/login.php</t>
+  </si>
+  <si>
     <t>496.html</t>
   </si>
   <si>
+    <t>https://www.ligo.co.uk/customer/account/login/</t>
+  </si>
+  <si>
     <t>497.html</t>
   </si>
   <si>
+    <t>https://www.att.com/my/#/login</t>
+  </si>
+  <si>
     <t>498.html</t>
   </si>
   <si>
+    <t>https://www.newtechindustries.com/login.php</t>
+  </si>
+  <si>
     <t>499.html</t>
   </si>
   <si>
+    <t>http://makeavoice.com/v2/</t>
+  </si>
+  <si>
     <t>500.html</t>
+  </si>
+  <si>
+    <t>http://www.homephonesonline.co.uk/myaccount/login.htm?ReturnUrl=%2fmyaccount%2fdefault.aspx</t>
+  </si>
+  <si>
+    <t>501.html</t>
+  </si>
+  <si>
+    <t>https://accounts.worldsim.com/Customer/Login.aspx</t>
+  </si>
+  <si>
+    <t>502.html</t>
+  </si>
+  <si>
+    <t>https://www.jammer-store.com/login/</t>
+  </si>
+  <si>
+    <t>503.html</t>
+  </si>
+  <si>
+    <t>https://www.nobelcom.com/myaccount/login.htm</t>
+  </si>
+  <si>
+    <t>504.html</t>
+  </si>
+  <si>
+    <t>https://www.comfi.com/reg/?l=/my-account/</t>
+  </si>
+  <si>
+    <t>505.html</t>
+  </si>
+  <si>
+    <t>http://callingcards.com/shopping/recharge_login.asp?GUID=44ACEEA92F8CA641B850014B576FF229</t>
+  </si>
+  <si>
+    <t>506.html</t>
+  </si>
+  <si>
+    <t>https://www.etechparts.com/customer/account/login/</t>
+  </si>
+  <si>
+    <t>507.html</t>
+  </si>
+  <si>
+    <t>https://www.callingcardplus.com/LogIn.asp</t>
+  </si>
+  <si>
+    <t>508.html</t>
+  </si>
+  <si>
+    <t>https://www.speedypin.com/sign-in.html?destination=https://www.speedypin.com/cust_account.html</t>
+  </si>
+  <si>
+    <t>509.html</t>
+  </si>
+  <si>
+    <t>https://mobilecaller.com/account/login</t>
+  </si>
+  <si>
+    <t>510.html</t>
+  </si>
+  <si>
+    <t>http://portal.piicomm.ca:8080/Login.aspx?ReturnUrl=default.asp</t>
+  </si>
+  <si>
+    <t>511.html</t>
+  </si>
+  <si>
+    <t>512.html</t>
+  </si>
+  <si>
+    <t>https://www.cricketwireless.com/myaccount.html#/login/1</t>
+  </si>
+  <si>
+    <t>513.html</t>
+  </si>
+  <si>
+    <t>https://www.youmail.com/login/signin?m=300</t>
+  </si>
+  <si>
+    <t>514.html</t>
+  </si>
+  <si>
+    <t>https://www.mophie.com/shop/customer/account/login</t>
+  </si>
+  <si>
+    <t>515.html</t>
+  </si>
+  <si>
+    <t>https://gsmserver.com/</t>
+  </si>
+  <si>
+    <t>516.html</t>
+  </si>
+  <si>
+    <t>https://www.repeaterstore.com/account/login</t>
+  </si>
+  <si>
+    <t>517.html</t>
+  </si>
+  <si>
+    <t>https://www.mazumamobile.com/sell_mobile_phone?action=login</t>
+  </si>
+  <si>
+    <t>518.html</t>
+  </si>
+  <si>
+    <t>https://www.sprint.com/</t>
+  </si>
+  <si>
+    <t>519.html</t>
+  </si>
+  <si>
+    <t>https://shop.icracked.com/account/login#</t>
+  </si>
+  <si>
+    <t>520.html</t>
+  </si>
+  <si>
+    <t>https://www.cellularoutfitter.com/account/login</t>
+  </si>
+  <si>
+    <t>521.html</t>
+  </si>
+  <si>
+    <t>https://www.wilsonamplifiers.com/login.php?from=account.php%3Faction%3D</t>
+  </si>
+  <si>
+    <t>522.html</t>
+  </si>
+  <si>
+    <t>https://www.rokform.com/account/login</t>
+  </si>
+  <si>
+    <t>523.html</t>
+  </si>
+  <si>
+    <t>http://www.cellsea.com/user/login/form</t>
+  </si>
+  <si>
+    <t>524.html</t>
+  </si>
+  <si>
+    <t>https://www.gadgetsalvation.com/</t>
+  </si>
+  <si>
+    <t>525.html</t>
+  </si>
+  <si>
+    <t>https://multi-com.eu/,client,itlskel_client_pgid,login.html</t>
+  </si>
+  <si>
+    <t>526.html</t>
+  </si>
+  <si>
+    <t>https://www.itsworthmore.com/</t>
+  </si>
+  <si>
+    <t>527.html</t>
+  </si>
+  <si>
+    <t>https://glyde.com/accounts/login</t>
+  </si>
+  <si>
+    <t>528.html</t>
+  </si>
+  <si>
+    <t>https://www.usell.com/</t>
+  </si>
+  <si>
+    <t>529.html</t>
+  </si>
+  <si>
+    <t>https://www.cellcorner.com/xshp/home.php</t>
+  </si>
+  <si>
+    <t>530.html</t>
+  </si>
+  <si>
+    <t>https://www.cellularabroad.com/xcart/secure_login.php</t>
+  </si>
+  <si>
+    <t>531.html</t>
+  </si>
+  <si>
+    <t>https://maxback.com/Login.aspx?ReturnUrl=%2f</t>
+  </si>
+  <si>
+    <t>532.html</t>
+  </si>
+  <si>
+    <t>https://www.puretalkusa.com/account/login</t>
+  </si>
+  <si>
+    <t>533.html</t>
+  </si>
+  <si>
+    <t>https://www.alternativewireless.com/login.php</t>
+  </si>
+  <si>
+    <t>534.html</t>
+  </si>
+  <si>
+    <t>535.html</t>
+  </si>
+  <si>
+    <t>https://www.unlockbase.com/login.php</t>
+  </si>
+  <si>
+    <t>536.html</t>
+  </si>
+  <si>
+    <t>https://www.xtremeguard.com/login.asp</t>
+  </si>
+  <si>
+    <t>537.html</t>
+  </si>
+  <si>
+    <t>https://www.thesignaljammer.com/login.php</t>
+  </si>
+  <si>
+    <t>538.html</t>
+  </si>
+  <si>
+    <t>https://www.onesimcard.com/telestial-account/</t>
+  </si>
+  <si>
+    <t>539.html</t>
+  </si>
+  <si>
+    <t>https://directpage.com/customer/account/login/</t>
+  </si>
+  <si>
+    <t>540.html</t>
+  </si>
+  <si>
+    <t>541.html</t>
+  </si>
+  <si>
+    <t>https://www.radioworld.co.uk/account/login</t>
+  </si>
+  <si>
+    <t>542.html</t>
+  </si>
+  <si>
+    <t>https://elecraft.com/account/login</t>
+  </si>
+  <si>
+    <t>543.html</t>
+  </si>
+  <si>
+    <t>https://www.rtsystemsinc.com/login.asp</t>
+  </si>
+  <si>
+    <t>544.html</t>
+  </si>
+  <si>
+    <t>https://www.hamradiolicenseexam.com/login.htm</t>
+  </si>
+  <si>
+    <t>545.html</t>
+  </si>
+  <si>
+    <t>https://www.bhi-ltd.com/log-in.html</t>
+  </si>
+  <si>
+    <t>546.html</t>
+  </si>
+  <si>
+    <t>http://www.inrad.net/home.php</t>
+  </si>
+  <si>
+    <t>547.html</t>
+  </si>
+  <si>
+    <t>https://www.argentdata.com/catalog/login.php?osCsid=Ygy9J8XbXwUoAv5K9oASc2</t>
+  </si>
+  <si>
+    <t>548.html</t>
+  </si>
+  <si>
+    <t>hamstation.com</t>
+  </si>
+  <si>
+    <t>549.html</t>
+  </si>
+  <si>
+    <t>https://american-milspec.com/signin.aspx?returnurl=%2F</t>
+  </si>
+  <si>
+    <t>550.html</t>
+  </si>
+  <si>
+    <t>https://hangar18surplus.com/login.php</t>
+  </si>
+  <si>
+    <t>551.html</t>
+  </si>
+  <si>
+    <t>https://www.dxengineering.com/login?returnURL=%2F</t>
+  </si>
+  <si>
+    <t>552.html</t>
+  </si>
+  <si>
+    <t>https://www.moonraker.eu/customer/account/login/referer/aHR0cHM6Ly93d3cubW9vbnJha2VyLmV1Lz9fX19TSUQ9VQ,,/</t>
+  </si>
+  <si>
+    <t>553.html</t>
+  </si>
+  <si>
+    <t>https://www.jpole-antenna.com/my-account/</t>
+  </si>
+  <si>
+    <t>554.html</t>
+  </si>
+  <si>
+    <t>https://www.m2inc.com/login.php?from=account.php%3Faction%3D</t>
+  </si>
+  <si>
+    <t>555.html</t>
+  </si>
+  <si>
+    <t>https://mgs4u.com/my-account/</t>
+  </si>
+  <si>
+    <t>556.html</t>
+  </si>
+  <si>
+    <t>https://www.wellbrook.uk.com/loopantennas/index.php?route=account/login</t>
+  </si>
+  <si>
+    <t>557.html</t>
+  </si>
+  <si>
+    <t>https://isotronantennas.com/index.php?main_page=login&amp;zenid=p19a8l4oumsp1itkqtebtrqa61</t>
+  </si>
+  <si>
+    <t>558.html</t>
+  </si>
+  <si>
+    <t>http://gapantenna.com/my-account/</t>
+  </si>
+  <si>
+    <t>559.html</t>
+  </si>
+  <si>
+    <t>https://primefocusantenna.com/index.php?main_page=login</t>
+  </si>
+  <si>
+    <t>560.html</t>
+  </si>
+  <si>
+    <t>https://www.wearecb.com/login.html?return_url=index.php</t>
+  </si>
+  <si>
+    <t>561.html</t>
+  </si>
+  <si>
+    <t>https://www.kcb.co.uk/shop2/contents/en-uk/login.html</t>
+  </si>
+  <si>
+    <t>562.html</t>
+  </si>
+  <si>
+    <t>https://www.cbradiosplus.com/login.asp</t>
+  </si>
+  <si>
+    <t>563.html</t>
+  </si>
+  <si>
+    <t>http://www.4x4cb.com/public/mylogin.cfm</t>
+  </si>
+  <si>
+    <t>564.html</t>
+  </si>
+  <si>
+    <t>https://customcbradios.auctivacommerce.com/Login.aspx?ReturnUrl=%2f</t>
+  </si>
+  <si>
+    <t>565.html</t>
+  </si>
+  <si>
+    <t>566.html</t>
+  </si>
+  <si>
+    <t>https://www.xm-radio-satellite.com/login.php?from=account.php%3Faction%3D</t>
+  </si>
+  <si>
+    <t>567.html</t>
+  </si>
+  <si>
+    <t>https://www.tss-radio.com/customer/account/login/referer/aHR0cHM6Ly93d3cudHNzLXJhZGlvLmNvbS9jdXN0b21lci9hY2NvdW50L2luZGV4Lw,,/</t>
+  </si>
+  <si>
+    <t>568.html</t>
+  </si>
+  <si>
+    <t>https://myradiostore.com/login.php?from=account.php%3Faction%3D</t>
+  </si>
+  <si>
+    <t>569.html</t>
+  </si>
+  <si>
+    <t>https://www.thetubestore.com/sca-dev-kilimanjaro/checkout.ssp?is=login&amp;login=T&amp;fragment=login-register#login-register</t>
+  </si>
+  <si>
+    <t>570.html</t>
+  </si>
+  <si>
+    <t>https://www.upscaleaudio.com/account/login</t>
+  </si>
+  <si>
+    <t>571.html</t>
+  </si>
+  <si>
+    <t>https://tubedepot.com/login</t>
+  </si>
+  <si>
+    <t>572.html</t>
+  </si>
+  <si>
+    <t>https://powerwerx.com/login</t>
+  </si>
+  <si>
+    <t>573.html</t>
+  </si>
+  <si>
+    <t>https://www.rfparts.com/customer/account/login/</t>
+  </si>
+  <si>
+    <t>574.html</t>
+  </si>
+  <si>
+    <t>https://www.minikits.com.au/index.php?route=account/login</t>
+  </si>
+  <si>
+    <t>575.html</t>
+  </si>
+  <si>
+    <t>https://www.mercurymagnetics.com/my-account/</t>
+  </si>
+  <si>
+    <t>576.html</t>
+  </si>
+  <si>
+    <t>https://www.eurotubes.com/store/pc/Checkout.asp?cmode=1</t>
+  </si>
+  <si>
+    <t>577.html</t>
+  </si>
+  <si>
+    <t>https://www.kcanostubes.com/user</t>
+  </si>
+  <si>
+    <t>578.html</t>
+  </si>
+  <si>
+    <t>https://vacuumtubesinc.com/index.php/customer/account/login/</t>
+  </si>
+  <si>
+    <t>579.html</t>
+  </si>
+  <si>
+    <t>https://www.nosvacuumtubes.net/my-account/</t>
+  </si>
+  <si>
+    <t>580.html</t>
+  </si>
+  <si>
+    <t>https://www.tubeman.com/index.php?l=account</t>
+  </si>
+  <si>
+    <t>581.html</t>
+  </si>
+  <si>
+    <t>https://harbachelectronics.com/my-account/</t>
+  </si>
+  <si>
+    <t>582.html</t>
+  </si>
+  <si>
+    <t>https://store.qkits.com/customer/account/login/</t>
+  </si>
+  <si>
+    <t>583.html</t>
+  </si>
+  <si>
+    <t>https://www.langrex.co.uk/my-account/</t>
+  </si>
+  <si>
+    <t>584.html</t>
+  </si>
+  <si>
+    <t>https://www.scannermaster.com/login.asp</t>
+  </si>
+  <si>
+    <t>585.html</t>
+  </si>
+  <si>
+    <t>https://www.bearcatscanner.com/login/?return_url=index.php</t>
+  </si>
+  <si>
+    <t>586.html</t>
+  </si>
+  <si>
+    <t>587.html</t>
+  </si>
+  <si>
+    <t>588.html</t>
+  </si>
+  <si>
+    <t>589.html</t>
+  </si>
+  <si>
+    <t>590.html</t>
+  </si>
+  <si>
+    <t>591.html</t>
+  </si>
+  <si>
+    <t>592.html</t>
+  </si>
+  <si>
+    <t>593.html</t>
+  </si>
+  <si>
+    <t>594.html</t>
+  </si>
+  <si>
+    <t>595.html</t>
+  </si>
+  <si>
+    <t>596.html</t>
+  </si>
+  <si>
+    <t>597.html</t>
+  </si>
+  <si>
+    <t>598.html</t>
+  </si>
+  <si>
+    <t>599.html</t>
+  </si>
+  <si>
+    <t>600.html</t>
   </si>
 </sst>
 </file>
@@ -6862,181 +7495,1011 @@
       <c r="A472" s="10" t="s">
         <v>933</v>
       </c>
-      <c r="B472" s="13"/>
+      <c r="B472" s="4" t="s">
+        <v>934</v>
+      </c>
     </row>
     <row r="473">
       <c r="A473" s="10" t="s">
-        <v>934</v>
-      </c>
-      <c r="B473" s="13"/>
+        <v>935</v>
+      </c>
+      <c r="B473" s="4" t="s">
+        <v>936</v>
+      </c>
     </row>
     <row r="474">
       <c r="A474" s="10" t="s">
-        <v>935</v>
-      </c>
-      <c r="B474" s="13"/>
+        <v>937</v>
+      </c>
+      <c r="B474" s="4" t="s">
+        <v>938</v>
+      </c>
     </row>
     <row r="475">
       <c r="A475" s="10" t="s">
-        <v>936</v>
-      </c>
-      <c r="B475" s="13"/>
+        <v>939</v>
+      </c>
+      <c r="B475" s="4" t="s">
+        <v>940</v>
+      </c>
     </row>
     <row r="476">
       <c r="A476" s="10" t="s">
-        <v>937</v>
-      </c>
-      <c r="B476" s="13"/>
+        <v>941</v>
+      </c>
+      <c r="B476" s="4" t="s">
+        <v>942</v>
+      </c>
     </row>
     <row r="477">
       <c r="A477" s="10" t="s">
-        <v>938</v>
-      </c>
-      <c r="B477" s="13"/>
+        <v>943</v>
+      </c>
+      <c r="B477" s="4" t="s">
+        <v>944</v>
+      </c>
     </row>
     <row r="478">
       <c r="A478" s="10" t="s">
-        <v>939</v>
-      </c>
-      <c r="B478" s="13"/>
+        <v>945</v>
+      </c>
+      <c r="B478" s="4" t="s">
+        <v>946</v>
+      </c>
     </row>
     <row r="479">
       <c r="A479" s="10" t="s">
-        <v>940</v>
-      </c>
-      <c r="B479" s="13"/>
+        <v>947</v>
+      </c>
+      <c r="B479" s="4" t="s">
+        <v>948</v>
+      </c>
     </row>
     <row r="480">
       <c r="A480" s="10" t="s">
-        <v>941</v>
-      </c>
-      <c r="B480" s="13"/>
+        <v>949</v>
+      </c>
+      <c r="B480" s="4" t="s">
+        <v>950</v>
+      </c>
     </row>
     <row r="481">
       <c r="A481" s="10" t="s">
-        <v>942</v>
-      </c>
-      <c r="B481" s="13"/>
+        <v>951</v>
+      </c>
+      <c r="B481" s="4" t="s">
+        <v>952</v>
+      </c>
     </row>
     <row r="482">
       <c r="A482" s="10" t="s">
-        <v>943</v>
-      </c>
-      <c r="B482" s="13"/>
+        <v>953</v>
+      </c>
+      <c r="B482" s="4" t="s">
+        <v>954</v>
+      </c>
     </row>
     <row r="483">
       <c r="A483" s="10" t="s">
-        <v>944</v>
-      </c>
-      <c r="B483" s="13"/>
+        <v>955</v>
+      </c>
+      <c r="B483" s="4" t="s">
+        <v>956</v>
+      </c>
     </row>
     <row r="484">
       <c r="A484" s="10" t="s">
-        <v>945</v>
-      </c>
-      <c r="B484" s="13"/>
+        <v>957</v>
+      </c>
+      <c r="B484" s="4" t="s">
+        <v>958</v>
+      </c>
     </row>
     <row r="485">
       <c r="A485" s="10" t="s">
-        <v>946</v>
-      </c>
-      <c r="B485" s="13"/>
+        <v>959</v>
+      </c>
+      <c r="B485" s="4" t="s">
+        <v>960</v>
+      </c>
     </row>
     <row r="486">
       <c r="A486" s="10" t="s">
-        <v>947</v>
-      </c>
-      <c r="B486" s="13"/>
+        <v>961</v>
+      </c>
+      <c r="B486" s="4" t="s">
+        <v>962</v>
+      </c>
     </row>
     <row r="487">
       <c r="A487" s="10" t="s">
-        <v>948</v>
-      </c>
-      <c r="B487" s="13"/>
+        <v>963</v>
+      </c>
+      <c r="B487" s="4" t="s">
+        <v>964</v>
+      </c>
     </row>
     <row r="488">
       <c r="A488" s="10" t="s">
-        <v>949</v>
-      </c>
-      <c r="B488" s="13"/>
+        <v>965</v>
+      </c>
+      <c r="B488" s="4" t="s">
+        <v>966</v>
+      </c>
     </row>
     <row r="489">
       <c r="A489" s="10" t="s">
-        <v>950</v>
-      </c>
-      <c r="B489" s="13"/>
+        <v>967</v>
+      </c>
+      <c r="B489" s="4" t="s">
+        <v>968</v>
+      </c>
     </row>
     <row r="490">
       <c r="A490" s="10" t="s">
-        <v>951</v>
-      </c>
-      <c r="B490" s="13"/>
+        <v>969</v>
+      </c>
+      <c r="B490" s="4" t="s">
+        <v>970</v>
+      </c>
     </row>
     <row r="491">
       <c r="A491" s="10" t="s">
-        <v>952</v>
-      </c>
-      <c r="B491" s="13"/>
+        <v>971</v>
+      </c>
+      <c r="B491" s="4" t="s">
+        <v>972</v>
+      </c>
     </row>
     <row r="492">
       <c r="A492" s="10" t="s">
-        <v>953</v>
-      </c>
-      <c r="B492" s="13"/>
+        <v>973</v>
+      </c>
+      <c r="B492" s="4" t="s">
+        <v>974</v>
+      </c>
     </row>
     <row r="493">
       <c r="A493" s="10" t="s">
-        <v>954</v>
-      </c>
-      <c r="B493" s="13"/>
+        <v>975</v>
+      </c>
+      <c r="B493" s="4" t="s">
+        <v>976</v>
+      </c>
     </row>
     <row r="494">
       <c r="A494" s="10" t="s">
-        <v>955</v>
-      </c>
-      <c r="B494" s="13"/>
+        <v>977</v>
+      </c>
+      <c r="B494" s="4" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="495">
       <c r="A495" s="10" t="s">
-        <v>956</v>
-      </c>
-      <c r="B495" s="13"/>
+        <v>979</v>
+      </c>
+      <c r="B495" s="4" t="s">
+        <v>980</v>
+      </c>
     </row>
     <row r="496">
       <c r="A496" s="10" t="s">
-        <v>957</v>
-      </c>
-      <c r="B496" s="13"/>
+        <v>981</v>
+      </c>
+      <c r="B496" s="4" t="s">
+        <v>982</v>
+      </c>
     </row>
     <row r="497">
       <c r="A497" s="10" t="s">
-        <v>958</v>
-      </c>
-      <c r="B497" s="13"/>
+        <v>983</v>
+      </c>
+      <c r="B497" s="4" t="s">
+        <v>984</v>
+      </c>
     </row>
     <row r="498">
       <c r="A498" s="10" t="s">
-        <v>959</v>
-      </c>
-      <c r="B498" s="13"/>
+        <v>985</v>
+      </c>
+      <c r="B498" s="4" t="s">
+        <v>986</v>
+      </c>
     </row>
     <row r="499">
       <c r="A499" s="10" t="s">
-        <v>960</v>
-      </c>
-      <c r="B499" s="13"/>
+        <v>987</v>
+      </c>
+      <c r="B499" s="4" t="s">
+        <v>988</v>
+      </c>
     </row>
     <row r="500">
       <c r="A500" s="10" t="s">
-        <v>961</v>
-      </c>
-      <c r="B500" s="13"/>
+        <v>989</v>
+      </c>
+      <c r="B500" s="4" t="s">
+        <v>990</v>
+      </c>
     </row>
     <row r="501">
       <c r="A501" s="10" t="s">
-        <v>962</v>
-      </c>
-      <c r="B501" s="13"/>
+        <v>991</v>
+      </c>
+      <c r="B501" s="4" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" s="10" t="s">
+        <v>993</v>
+      </c>
+      <c r="B502" s="4" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" s="10" t="s">
+        <v>995</v>
+      </c>
+      <c r="B503" s="4" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" s="10" t="s">
+        <v>997</v>
+      </c>
+      <c r="B504" s="4" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" s="10" t="s">
+        <v>999</v>
+      </c>
+      <c r="B505" s="4" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" s="10" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B506" s="4" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" s="10" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B507" s="4" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" s="10" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B508" s="4" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" s="10" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B509" s="4" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" s="10" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B510" s="4" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" s="10" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B511" s="4" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" s="10" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B512" s="4" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" s="10" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B513" s="4" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" s="10" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B514" s="4" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" s="10" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B515" s="4" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" s="10" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B516" s="4" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" s="10" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B517" s="4" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" s="10" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B518" s="4" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" s="10" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B519" s="4" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" s="10" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B520" s="4" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" s="10" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B521" s="4" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" s="10" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B522" s="4" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" s="10" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B523" s="4" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" s="10" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B524" s="4" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" s="10" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B525" s="4" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" s="10" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B526" s="4" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" s="10" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B527" s="4" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" s="10" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B528" s="4" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" s="10" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B529" s="4" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" s="10" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B530" s="4" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" s="10" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B531" s="4" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" s="10" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B532" s="4" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" s="10" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B533" s="4" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" s="10" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B534" s="4" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" s="10" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B535" s="4" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" s="10" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B536" s="4" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" s="10" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B537" s="4" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" s="10" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B538" s="4" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" s="10" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B539" s="4" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" s="10" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B540" s="4" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" s="10" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B541" s="4" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" s="10" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B542" s="4" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" s="10" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B543" s="4" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" s="10" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B544" s="4" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" s="10" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B545" s="4" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" s="10" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B546" s="4" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" s="10" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B547" s="4" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" s="10" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B548" s="4" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" s="10" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B549" s="4" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" s="10" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B550" s="4" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" s="10" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B551" s="4" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" s="10" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B552" s="4" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" s="10" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B553" s="4" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" s="10" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B554" s="4" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" s="10" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B555" s="4" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" s="10" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B556" s="4" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" s="10" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B557" s="4" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" s="10" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B558" s="4" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" s="10" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B559" s="4" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" s="10" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B560" s="4" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" s="10" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B561" s="4" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" s="10" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B562" s="4" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" s="10" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B563" s="4" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" s="10" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B564" s="4" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" s="10" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B565" s="4" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" s="10" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B566" s="4" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" s="10" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B567" s="4" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" s="10" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B568" s="4" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" s="10" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B569" s="4" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" s="10" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B570" s="4" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" s="10" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B571" s="4" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" s="10" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B572" s="4" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" s="10" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B573" s="4" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" s="10" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B574" s="4" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" s="10" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B575" s="4" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" s="10" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B576" s="4" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" s="10" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B577" s="4" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" s="10" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B578" s="4" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" s="10" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B579" s="4" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" s="10" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B580" s="4" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" s="10" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B581" s="4" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" s="10" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B582" s="4" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" s="10" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B583" s="4" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" s="10" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B584" s="4" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" s="10" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B585" s="4" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" s="10" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B586" s="4" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" s="10" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B587" s="13"/>
+    </row>
+    <row r="588">
+      <c r="A588" s="10" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B588" s="13"/>
+    </row>
+    <row r="589">
+      <c r="A589" s="10" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B589" s="13"/>
+    </row>
+    <row r="590">
+      <c r="A590" s="10" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B590" s="13"/>
+    </row>
+    <row r="591">
+      <c r="A591" s="10" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B591" s="13"/>
+    </row>
+    <row r="592">
+      <c r="A592" s="10" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B592" s="13"/>
+    </row>
+    <row r="593">
+      <c r="A593" s="10" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B593" s="13"/>
+    </row>
+    <row r="594">
+      <c r="A594" s="10" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B594" s="13"/>
+    </row>
+    <row r="595">
+      <c r="A595" s="10" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B595" s="13"/>
+    </row>
+    <row r="596">
+      <c r="A596" s="10" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B596" s="13"/>
+    </row>
+    <row r="597">
+      <c r="A597" s="10" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B597" s="13"/>
+    </row>
+    <row r="598">
+      <c r="A598" s="10" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B598" s="13"/>
+    </row>
+    <row r="599">
+      <c r="A599" s="10" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B599" s="13"/>
+    </row>
+    <row r="600">
+      <c r="A600" s="10" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B600" s="13"/>
+    </row>
+    <row r="601">
+      <c r="A601" s="10" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B601" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -7509,7 +8972,122 @@
     <hyperlink r:id="rId467" ref="B469"/>
     <hyperlink r:id="rId468" ref="B470"/>
     <hyperlink r:id="rId469" ref="B471"/>
+    <hyperlink r:id="rId470" ref="B472"/>
+    <hyperlink r:id="rId471" ref="B473"/>
+    <hyperlink r:id="rId472" ref="B474"/>
+    <hyperlink r:id="rId473" ref="B475"/>
+    <hyperlink r:id="rId474" ref="B476"/>
+    <hyperlink r:id="rId475" ref="B477"/>
+    <hyperlink r:id="rId476" ref="B478"/>
+    <hyperlink r:id="rId477" ref="B479"/>
+    <hyperlink r:id="rId478" ref="B480"/>
+    <hyperlink r:id="rId479" ref="B481"/>
+    <hyperlink r:id="rId480" ref="B482"/>
+    <hyperlink r:id="rId481" ref="B483"/>
+    <hyperlink r:id="rId482" ref="B484"/>
+    <hyperlink r:id="rId483" ref="B485"/>
+    <hyperlink r:id="rId484" ref="B486"/>
+    <hyperlink r:id="rId485" ref="B487"/>
+    <hyperlink r:id="rId486" ref="B488"/>
+    <hyperlink r:id="rId487" ref="B489"/>
+    <hyperlink r:id="rId488" ref="B490"/>
+    <hyperlink r:id="rId489" ref="B491"/>
+    <hyperlink r:id="rId490" ref="B492"/>
+    <hyperlink r:id="rId491" ref="B493"/>
+    <hyperlink r:id="rId492" ref="B494"/>
+    <hyperlink r:id="rId493" ref="B495"/>
+    <hyperlink r:id="rId494" ref="B496"/>
+    <hyperlink r:id="rId495" ref="B497"/>
+    <hyperlink r:id="rId496" location="/login" ref="B498"/>
+    <hyperlink r:id="rId497" ref="B499"/>
+    <hyperlink r:id="rId498" ref="B500"/>
+    <hyperlink r:id="rId499" ref="B501"/>
+    <hyperlink r:id="rId500" ref="B502"/>
+    <hyperlink r:id="rId501" ref="B503"/>
+    <hyperlink r:id="rId502" ref="B504"/>
+    <hyperlink r:id="rId503" ref="B505"/>
+    <hyperlink r:id="rId504" ref="B506"/>
+    <hyperlink r:id="rId505" ref="B507"/>
+    <hyperlink r:id="rId506" ref="B508"/>
+    <hyperlink r:id="rId507" ref="B509"/>
+    <hyperlink r:id="rId508" ref="B510"/>
+    <hyperlink r:id="rId509" ref="B511"/>
+    <hyperlink r:id="rId510" ref="B512"/>
+    <hyperlink r:id="rId511" location="/login/1" ref="B513"/>
+    <hyperlink r:id="rId512" ref="B514"/>
+    <hyperlink r:id="rId513" ref="B515"/>
+    <hyperlink r:id="rId514" ref="B516"/>
+    <hyperlink r:id="rId515" ref="B517"/>
+    <hyperlink r:id="rId516" ref="B518"/>
+    <hyperlink r:id="rId517" ref="B519"/>
+    <hyperlink r:id="rId518" ref="B520"/>
+    <hyperlink r:id="rId519" ref="B521"/>
+    <hyperlink r:id="rId520" ref="B522"/>
+    <hyperlink r:id="rId521" ref="B523"/>
+    <hyperlink r:id="rId522" ref="B524"/>
+    <hyperlink r:id="rId523" ref="B525"/>
+    <hyperlink r:id="rId524" ref="B526"/>
+    <hyperlink r:id="rId525" ref="B527"/>
+    <hyperlink r:id="rId526" ref="B528"/>
+    <hyperlink r:id="rId527" ref="B529"/>
+    <hyperlink r:id="rId528" ref="B530"/>
+    <hyperlink r:id="rId529" ref="B531"/>
+    <hyperlink r:id="rId530" ref="B532"/>
+    <hyperlink r:id="rId531" ref="B533"/>
+    <hyperlink r:id="rId532" ref="B534"/>
+    <hyperlink r:id="rId533" ref="B535"/>
+    <hyperlink r:id="rId534" ref="B536"/>
+    <hyperlink r:id="rId535" ref="B537"/>
+    <hyperlink r:id="rId536" ref="B538"/>
+    <hyperlink r:id="rId537" ref="B539"/>
+    <hyperlink r:id="rId538" ref="B540"/>
+    <hyperlink r:id="rId539" ref="B541"/>
+    <hyperlink r:id="rId540" ref="B542"/>
+    <hyperlink r:id="rId541" ref="B543"/>
+    <hyperlink r:id="rId542" ref="B544"/>
+    <hyperlink r:id="rId543" ref="B545"/>
+    <hyperlink r:id="rId544" ref="B546"/>
+    <hyperlink r:id="rId545" ref="B547"/>
+    <hyperlink r:id="rId546" ref="B548"/>
+    <hyperlink r:id="rId547" ref="B549"/>
+    <hyperlink r:id="rId548" ref="B550"/>
+    <hyperlink r:id="rId549" ref="B551"/>
+    <hyperlink r:id="rId550" ref="B552"/>
+    <hyperlink r:id="rId551" ref="B553"/>
+    <hyperlink r:id="rId552" ref="B554"/>
+    <hyperlink r:id="rId553" ref="B555"/>
+    <hyperlink r:id="rId554" ref="B556"/>
+    <hyperlink r:id="rId555" ref="B557"/>
+    <hyperlink r:id="rId556" ref="B558"/>
+    <hyperlink r:id="rId557" ref="B559"/>
+    <hyperlink r:id="rId558" ref="B560"/>
+    <hyperlink r:id="rId559" ref="B561"/>
+    <hyperlink r:id="rId560" ref="B562"/>
+    <hyperlink r:id="rId561" ref="B563"/>
+    <hyperlink r:id="rId562" ref="B564"/>
+    <hyperlink r:id="rId563" ref="B565"/>
+    <hyperlink r:id="rId564" ref="B566"/>
+    <hyperlink r:id="rId565" ref="B567"/>
+    <hyperlink r:id="rId566" ref="B568"/>
+    <hyperlink r:id="rId567" ref="B569"/>
+    <hyperlink r:id="rId568" location="login-register" ref="B570"/>
+    <hyperlink r:id="rId569" ref="B571"/>
+    <hyperlink r:id="rId570" ref="B572"/>
+    <hyperlink r:id="rId571" ref="B573"/>
+    <hyperlink r:id="rId572" ref="B574"/>
+    <hyperlink r:id="rId573" ref="B575"/>
+    <hyperlink r:id="rId574" ref="B576"/>
+    <hyperlink r:id="rId575" ref="B577"/>
+    <hyperlink r:id="rId576" ref="B578"/>
+    <hyperlink r:id="rId577" ref="B579"/>
+    <hyperlink r:id="rId578" ref="B580"/>
+    <hyperlink r:id="rId579" ref="B581"/>
+    <hyperlink r:id="rId580" ref="B582"/>
+    <hyperlink r:id="rId581" ref="B583"/>
+    <hyperlink r:id="rId582" ref="B584"/>
+    <hyperlink r:id="rId583" ref="B585"/>
+    <hyperlink r:id="rId584" ref="B586"/>
   </hyperlinks>
-  <drawing r:id="rId470"/>
+  <drawing r:id="rId585"/>
 </worksheet>
 </file>
</xml_diff>